<commit_message>
Import Aspirants functionality commit & Removed import from Employees section
</commit_message>
<xml_diff>
--- a/UI/ExamPortal/src/assets/user-template/userTemplate.xlsx
+++ b/UI/ExamPortal/src/assets/user-template/userTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8823C3E0-18E3-42CF-95EA-0691F82BC6BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8703999B-2806-4DF1-8957-0E6F42B48158}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,31 +20,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>middleName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>contact no.</t>
-  </si>
-  <si>
-    <t>email</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>Address 2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Pincode</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Nagpur</t>
+  </si>
+  <si>
+    <t>MUMBAI</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>Ramakant</t>
+  </si>
+  <si>
+    <t>Shyam</t>
+  </si>
+  <si>
+    <t>Chandel</t>
+  </si>
+  <si>
+    <t>ramakant.chandel@perficient.com</t>
+  </si>
+  <si>
+    <t>CurrentAddress1</t>
+  </si>
+  <si>
+    <t>CurrentAddress2</t>
+  </si>
+  <si>
+    <t>CurrentCity</t>
+  </si>
+  <si>
+    <t>CurrentStateId</t>
+  </si>
+  <si>
+    <t>CurrentPincode</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Interest</t>
+  </si>
+  <si>
+    <t>This is a note</t>
+  </si>
+  <si>
+    <t>HTML/CSS, Design</t>
+  </si>
+  <si>
+    <t>Madhya Pradesh</t>
+  </si>
+  <si>
+    <t>Magento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -67,13 +147,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -352,39 +440,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" customWidth="1"/>
+    <col min="15" max="16" width="13.85546875" customWidth="1"/>
+    <col min="17" max="17" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="1">
+        <v>440024</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="1">
+        <v>440024</v>
+      </c>
+      <c r="O2" s="1">
+        <v>9960160804</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2 M2" xr:uid="{2CAFC395-0934-4395-9CBB-BE0358669FC6}">
+      <formula1>"Maharashta, Delhi, Madhya Pradesh, Tamil Nadu"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2" xr:uid="{D85DBE8D-8B9C-4C74-BAC8-16F48DA684A6}">
+      <formula1>"AEM, .Net Technology, Magento, UI team, ALL, PHP Team"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{34C8AC8C-EAB2-4D88-82B4-38B061A90C56}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>